<commit_message>
Popravil izbirce, poravil predmet counter, naredil statistiko nad predmeti
</commit_message>
<xml_diff>
--- a/nasi_podatki/statistika_predmetov.xlsx
+++ b/nasi_podatki/statistika_predmetov.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
   <si>
     <t>Predmet</t>
   </si>
@@ -22,201 +22,201 @@
     <t>Pojavitev</t>
   </si>
   <si>
+    <t>'Glasbeni projekt /i/'</t>
+  </si>
+  <si>
+    <t>'Genetika /i/'</t>
+  </si>
+  <si>
     <t>'Nemščina II /i/'</t>
   </si>
   <si>
+    <t>'Izbrani šport /i/'</t>
+  </si>
+  <si>
+    <t>'Urejanje besedil /i/'</t>
+  </si>
+  <si>
+    <t>'Kemija v okolju /i/'</t>
+  </si>
+  <si>
+    <t>'Kaj nam govorijo umetnine /i/'</t>
+  </si>
+  <si>
+    <t>'Raziskovanje organizmov v domači okolici /i/'</t>
+  </si>
+  <si>
     <t>'Filozofija za otroke: Jaz in drugi /i/'</t>
   </si>
   <si>
-    <t>'Izbrani šport /i/'</t>
+    <t>'Verstva in etika 2 /i/'</t>
+  </si>
+  <si>
+    <t>'Likovno snovanje 2 /i/'</t>
+  </si>
+  <si>
+    <t>'Klekljanje II /i/'</t>
+  </si>
+  <si>
+    <t>'Gledališki klub /i/'</t>
+  </si>
+  <si>
+    <t>'Likovno snovanje 3 /i/'</t>
   </si>
   <si>
     <t>'Šport za sprostitev /i/'</t>
   </si>
   <si>
+    <t>'Obdelava gradiv: les /i/'</t>
+  </si>
+  <si>
+    <t>'Verstva in etika 1 /i/'</t>
+  </si>
+  <si>
+    <t>'Turistična vzgoja /i/'</t>
+  </si>
+  <si>
+    <t>'Literarni klub /i/'</t>
+  </si>
+  <si>
+    <t>'Francoščina II /i/'</t>
+  </si>
+  <si>
+    <t>'Klekljanje I /i/'</t>
+  </si>
+  <si>
+    <t>'Šport za zdravje /i/'</t>
+  </si>
+  <si>
+    <t>'Klekljanje III /i/'</t>
+  </si>
+  <si>
+    <t>'Poskusi v kemiji /i/'</t>
+  </si>
+  <si>
+    <t>'Nemščina III /i/'</t>
+  </si>
+  <si>
     <t>'Likovno snovanje 1 /i/'</t>
   </si>
   <si>
+    <t>'Sodobna priprava hrane /i/'</t>
+  </si>
+  <si>
+    <t>'Obdelava gradiv: umetne snovi /i/'</t>
+  </si>
+  <si>
+    <t>'Nemščina I /i/'</t>
+  </si>
+  <si>
+    <t>'Francoščina I /i/'</t>
+  </si>
+  <si>
+    <t>'Računalniška omrežja /i/'</t>
+  </si>
+  <si>
+    <t>'Šolsko novinarstvo /i/'</t>
+  </si>
+  <si>
+    <t>'Načini prehranjevanja /i/'</t>
+  </si>
+  <si>
+    <t>'Francoščina III /i/'</t>
+  </si>
+  <si>
     <t>'Rastline in človek /i/'</t>
   </si>
   <si>
+    <t>'Retorika /i/'</t>
+  </si>
+  <si>
+    <t>'Obdelava gradiv: kovine /i/'</t>
+  </si>
+  <si>
     <t>'Multimedia /i/'</t>
   </si>
   <si>
-    <t>'Retorika /i/'</t>
-  </si>
-  <si>
-    <t>'Sodobna priprava hrane /i/'</t>
-  </si>
-  <si>
-    <t>'Nemščina I /i/'</t>
-  </si>
-  <si>
-    <t>'Nemščina III /i/'</t>
-  </si>
-  <si>
-    <t>'Šport za zdravje /i/'</t>
+    <t>'Daljnogledi in planeti /i/'</t>
   </si>
   <si>
     <t>'Organizmi v naravi in umetnem okolju /i/'</t>
   </si>
   <si>
-    <t>'Likovno snovanje 3 /i/'</t>
-  </si>
-  <si>
-    <t>'Klekljanje II /i/'</t>
-  </si>
-  <si>
-    <t>'Genetika /i/'</t>
-  </si>
-  <si>
-    <t>'Klekljanje I /i/'</t>
-  </si>
-  <si>
-    <t>'Francoščina I /i/'</t>
-  </si>
-  <si>
-    <t>'Računalniška omrežja /i/'</t>
-  </si>
-  <si>
-    <t>'Likovno snovanje 2 /i/'</t>
-  </si>
-  <si>
-    <t>'Glasbeni projekt /i/'</t>
-  </si>
-  <si>
-    <t>'Poskusi v kemiji /i/'</t>
-  </si>
-  <si>
-    <t>'Kemija v okolju /i/'</t>
-  </si>
-  <si>
-    <t>'Francoščina II /i/'</t>
-  </si>
-  <si>
-    <t>'Gledališki klub /i/'</t>
-  </si>
-  <si>
-    <t>'Obdelava gradiv: les /i/'</t>
-  </si>
-  <si>
-    <t>'Urejanje besedil /i/'</t>
-  </si>
-  <si>
-    <t>'Verstva in etika 1 /i/'</t>
-  </si>
-  <si>
-    <t>'Klekljanje III /i/'</t>
-  </si>
-  <si>
-    <t>'Verstva in etika 2 /i/'</t>
-  </si>
-  <si>
-    <t>'Obdelava gradiv: umetne snovi /i/'</t>
-  </si>
-  <si>
-    <t>'Načini prehranjevanja /i/'</t>
-  </si>
-  <si>
-    <t>'Kaj nam govorijo umetnine /i/'</t>
-  </si>
-  <si>
-    <t>'Francoščina III /i/'</t>
-  </si>
-  <si>
-    <t>'Literarni klub /i/'</t>
-  </si>
-  <si>
-    <t>'Turistična vzgoja /i/'</t>
-  </si>
-  <si>
-    <t>'Daljnogledi in planeti /i/'</t>
-  </si>
-  <si>
-    <t>'Šolsko novinarstvo /i/'</t>
-  </si>
-  <si>
-    <t>'Raziskovanje organizmov v domači okolici /i/'</t>
-  </si>
-  <si>
-    <t>'Obdelava gradiv: kovine /i/'</t>
+    <t>'Zvezde in vesolje /i/'</t>
+  </si>
+  <si>
+    <t>'Elektrotehnika /i/'</t>
+  </si>
+  <si>
+    <t>'Vezenje: Osnovni vbodi in tehnike vezenja /i/'</t>
+  </si>
+  <si>
+    <t>'Starinski in družabni plesi /i/'</t>
+  </si>
+  <si>
+    <t>'Italijanščina III /i/'</t>
+  </si>
+  <si>
+    <t>'Čebelarstvo /i/'</t>
+  </si>
+  <si>
+    <t>'Sonce Luna in Zemlja /i/'</t>
+  </si>
+  <si>
+    <t>'Vezenje: Slikarski marjetični in gobelinski vbodi (i)'</t>
   </si>
   <si>
     <t>'Elektronika z robotiko /i/'</t>
   </si>
   <si>
-    <t>'Italijanščina III /i/'</t>
-  </si>
-  <si>
     <t>'Ples /i/'</t>
   </si>
   <si>
+    <t>'Italijanščina II /i/'</t>
+  </si>
+  <si>
     <t>'Italijanščina I /i/'</t>
   </si>
   <si>
-    <t>'Čebelarstvo /i/'</t>
-  </si>
-  <si>
     <t>'Ljudski plesi /i/'</t>
   </si>
   <si>
-    <t>'Italijanščina II /i/'</t>
-  </si>
-  <si>
-    <t>'Starinski in družabni plesi /i/'</t>
-  </si>
-  <si>
-    <t>'Zvezde in vesolje /i/'</t>
-  </si>
-  <si>
-    <t>'Elektrotehnika /i/'</t>
-  </si>
-  <si>
-    <t>'Sonce Luna in Zemlja /i/'</t>
-  </si>
-  <si>
-    <t>'Vezenje: Slikarski marjetični in gobelinski vbodi (i)'</t>
-  </si>
-  <si>
-    <t>'Vezenje: Osnovni vbodi in tehnike vezenja /i/'</t>
+    <t>'Matematične delavnice 7 /i/'</t>
+  </si>
+  <si>
+    <t>'Matematične delavnice 8 /i/'</t>
   </si>
   <si>
     <t>'Raziskovanje domače okolice /i/'</t>
   </si>
   <si>
+    <t>'Matematične delavnice 9 /i/'</t>
+  </si>
+  <si>
     <t>'Odkrivajmo preteklost mojega kraja /i/'</t>
   </si>
   <si>
-    <t>'Matematične delavnice 7 /i/'</t>
-  </si>
-  <si>
-    <t>'Matematične delavnice 8 /i/'</t>
-  </si>
-  <si>
-    <t>'Matematične delavnice 9 /i/'</t>
+    <t>'Filozofija za otroke: Kritično mišljenje /i/'</t>
+  </si>
+  <si>
+    <t>'Glasbena dela /i/'</t>
+  </si>
+  <si>
+    <t>'Robotika v tehniki /i/'</t>
+  </si>
+  <si>
+    <t>'Televizija /i/'</t>
   </si>
   <si>
     <t>'Radio /i/'</t>
   </si>
   <si>
-    <t>'Televizija /i/'</t>
+    <t>'Filozofija za otroke: Etična raziskovanja /i/'</t>
   </si>
   <si>
     <t>'Ansambelska igra /i/'</t>
   </si>
   <si>
-    <t>'Filozofija za otroke: Kritično mišljenje /i/'</t>
-  </si>
-  <si>
-    <t>'Glasbena dela /i/'</t>
-  </si>
-  <si>
-    <t>'Robotika v tehniki /i/'</t>
-  </si>
-  <si>
-    <t>'Filozofija za otroke: Etična raziskovanja /i/'</t>
-  </si>
-  <si>
     <t>'Verstva in etika 3 /i/'</t>
   </si>
   <si>
@@ -229,6 +229,12 @@
     <t>'Šahovske osnove /i/'</t>
   </si>
   <si>
+    <t>'Kemija v življenju /i/'</t>
+  </si>
+  <si>
+    <t>'Državljanska kultura /i/'</t>
+  </si>
+  <si>
     <t>'Življenje človeka na zemlji /i/'</t>
   </si>
   <si>
@@ -238,96 +244,90 @@
     <t>'Kmetijska dela /i/'</t>
   </si>
   <si>
-    <t>'Državljanska kultura /i/'</t>
+    <t>'Varstvo pred naravnimi in drugimi nesrečami /i/'</t>
   </si>
   <si>
     <t>'Informacijsko opismenjevanje /i/'</t>
   </si>
   <si>
-    <t>'Varstvo pred naravnimi in drugimi nesrečami /i/'</t>
-  </si>
-  <si>
-    <t>'Kemija v življenju /i/'</t>
-  </si>
-  <si>
     <t>'Logika I /i/'</t>
   </si>
   <si>
+    <t>'Življenje upodobljeno v umetnosti /i/'</t>
+  </si>
+  <si>
     <t>'Oblika in slog /i/'</t>
   </si>
   <si>
-    <t>'Življenje upodobljeno v umetnosti /i/'</t>
-  </si>
-  <si>
     <t>'Hrvaščina I /i/'</t>
   </si>
   <si>
+    <t>'Projekti iz fizike in tehnike /i/'</t>
+  </si>
+  <si>
     <t>'Okoljska vzgoja I /i/'</t>
   </si>
   <si>
-    <t>'Projekti iz fizike in tehnike /i/'</t>
-  </si>
-  <si>
     <t>'Šahovsko kombiniranje /i/'</t>
   </si>
   <si>
+    <t>'Španščina II /i/'</t>
+  </si>
+  <si>
+    <t>'Kitajščina I /i/'</t>
+  </si>
+  <si>
     <t>'Španščina I /i/'</t>
   </si>
   <si>
-    <t>'Španščina II /i/'</t>
-  </si>
-  <si>
-    <t>'Kitajščina I /i/'</t>
-  </si>
-  <si>
     <t>'Šahovske strategije /i/'</t>
   </si>
   <si>
+    <t>'Španščina III /i/'</t>
+  </si>
+  <si>
     <t>'Logika II /i/'</t>
   </si>
   <si>
-    <t>'Španščina III /i/'</t>
-  </si>
-  <si>
     <t>'Angleščina I /i/'</t>
   </si>
   <si>
+    <t>'Angleščina II /i/'</t>
+  </si>
+  <si>
+    <t>'Projekti iz fizike in ekologije /i/'</t>
+  </si>
+  <si>
     <t>'Angleščina III /i/'</t>
   </si>
   <si>
-    <t>'Angleščina II /i/'</t>
-  </si>
-  <si>
-    <t>'Projekti iz fizike in ekologije /i/'</t>
+    <t>'Klaviatura in računalnik II /i/'</t>
+  </si>
+  <si>
+    <t>'Srečanja s kulturami in načini življenja /i/'</t>
   </si>
   <si>
     <t>'Klaviatura in računalnik I /i/'</t>
   </si>
   <si>
-    <t>'Klaviatura in računalnik II /i/'</t>
-  </si>
-  <si>
-    <t>'Srečanja s kulturami in načini življenja /i/'</t>
+    <t>'Ruščina II /i/'</t>
+  </si>
+  <si>
+    <t>'Ruščina I /i/'</t>
   </si>
   <si>
     <t>'Ruščina III /i/'</t>
   </si>
   <si>
-    <t>'Ruščina II /i/'</t>
-  </si>
-  <si>
-    <t>'Ruščina I /i/'</t>
-  </si>
-  <si>
     <t>'Risanje v geometriji in tehniki /i/'</t>
   </si>
   <si>
+    <t>'Okoljska vzgoja III /i/'</t>
+  </si>
+  <si>
     <t>'Okoljska vzgoja II /i/'</t>
   </si>
   <si>
-    <t>'Okoljska vzgoja III /i/'</t>
-  </si>
-  <si>
     <t>'Sodobno kmetijstvo /i/'</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>'Logika III /i/'</t>
   </si>
   <si>
+    <t>'Latinščina I /i/'</t>
+  </si>
+  <si>
     <t>'Latinščina II /i/'</t>
   </si>
   <si>
-    <t>'Latinščina I /i/'</t>
-  </si>
-  <si>
     <t>'Sodobnosti z razsežnostmi dediščine /i/'</t>
   </si>
   <si>
@@ -376,13 +376,10 @@
     <t>'Kulturna dediščina in načini življenja /i/'</t>
   </si>
   <si>
-    <t xml:space="preserve"> Podružnica Zavrč'</t>
+    <t>'Madžarščina I /i/'</t>
   </si>
   <si>
     <t>'Madžarščina II /i/'</t>
-  </si>
-  <si>
-    <t>'Madžarščina I /i/'</t>
   </si>
 </sst>
 </file>
@@ -718,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -747,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>196</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -755,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>4430</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -763,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>4380</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -771,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>2888</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -779,7 +776,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>519</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -787,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>3363</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -795,7 +792,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>859</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -803,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>3037</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -811,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>3317</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -819,7 +816,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>3045</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -827,7 +824,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>4431</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -835,7 +832,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>690</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -843,7 +840,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>2652</v>
+        <v>417</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -851,7 +848,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>58</v>
+        <v>507</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -859,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>193</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -867,7 +864,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -875,7 +872,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>658</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -883,7 +880,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>3190</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -891,7 +888,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>2699</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -899,7 +896,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>468</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -907,7 +904,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>2288</v>
+        <v>520</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -915,7 +912,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>167</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -923,7 +920,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>617</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -931,7 +928,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>1659</v>
+        <v>407</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -939,7 +936,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>2520</v>
+        <v>468</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -947,7 +944,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>3224</v>
+        <v>442</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -955,7 +952,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>239</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -963,7 +960,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>41</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -971,7 +968,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>182</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -979,7 +976,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>932</v>
+        <v>444</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -987,7 +984,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="n">
-        <v>1758</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -995,7 +992,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>62</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1003,7 +1000,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>520</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1011,7 +1008,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1019,7 +1016,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>1578</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1027,7 +1024,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>483</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1035,7 +1032,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>978</v>
+        <v>463</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1043,7 +1040,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1051,7 +1048,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>693</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1059,7 +1056,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>275</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1067,7 +1064,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>336</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1075,7 +1072,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>960</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1083,7 +1080,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>419</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1091,7 +1088,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1099,7 +1096,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>192</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1107,7 +1104,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>384</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1115,7 +1112,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>368</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1123,7 +1120,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>446</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1131,7 +1128,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>330</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1139,7 +1136,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>926</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1147,7 +1144,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1155,7 +1152,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>146</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1163,7 +1160,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>171</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1171,7 +1168,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1179,7 +1176,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>264</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1187,7 +1184,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
-        <v>184</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1195,7 +1192,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
-        <v>160</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1203,7 +1200,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="n">
-        <v>370</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1211,7 +1208,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>550</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1219,7 +1216,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>654</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1227,7 +1224,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1235,7 +1232,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>296</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1243,7 +1240,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>519</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1251,7 +1248,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>127</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1259,7 +1256,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>173</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1267,7 +1264,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="n">
-        <v>188</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1275,7 +1272,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>346</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1283,7 +1280,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>312</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1291,7 +1288,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="n">
-        <v>489</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1299,7 +1296,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="n">
-        <v>349</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1307,7 +1304,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="n">
-        <v>102</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1315,7 +1312,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="n">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1323,7 +1320,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1331,7 +1328,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="n">
-        <v>234</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1339,7 +1336,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="n">
-        <v>410</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1347,7 +1344,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="n">
-        <v>152</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1355,7 +1352,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1363,7 +1360,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="n">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1371,7 +1368,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1379,7 +1376,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="n">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1387,7 +1384,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1395,7 +1392,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="n">
-        <v>103</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1403,7 +1400,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="n">
-        <v>523</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1411,7 +1408,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="n">
-        <v>424</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1419,7 +1416,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="n">
-        <v>9</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1427,7 +1424,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="n">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1435,7 +1432,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="n">
-        <v>39</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1443,7 +1440,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="n">
-        <v>323</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1451,7 +1448,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="n">
-        <v>307</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1459,7 +1456,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="n">
-        <v>372</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1467,7 +1464,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="n">
-        <v>330</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1475,7 +1472,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="n">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1483,7 +1480,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="n">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1491,7 +1488,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1499,7 +1496,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="n">
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1507,7 +1504,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1515,7 +1512,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1523,7 +1520,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="n">
-        <v>47</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1531,7 +1528,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="n">
-        <v>93</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1539,7 +1536,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="n">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1547,7 +1544,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1555,7 +1552,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1563,7 +1560,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1571,7 +1568,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1579,7 +1576,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1587,7 +1584,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1595,7 +1592,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1603,7 +1600,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="n">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1619,7 +1616,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1627,7 +1624,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1635,7 +1632,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1643,7 +1640,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1651,7 +1648,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1667,7 +1664,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1683,7 +1680,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="n">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1691,14 +1688,6 @@
         <v>121</v>
       </c>
       <c r="B121" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" t="s">
-        <v>122</v>
-      </c>
-      <c r="B122" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>